<commit_message>
update BookRecorder.xlsx and S007_ProgrammingGuide.docx
</commit_message>
<xml_diff>
--- a/반월도서관희망도서목록2019.xlsx
+++ b/반월도서관희망도서목록2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="JAN1" sheetId="3" r:id="rId1"/>
@@ -3307,7 +3307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3347,6 +3347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3425,7 +3431,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3498,9 +3504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -3512,6 +3515,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3845,15 +3857,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -4604,7 +4616,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4620,16 +4632,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>962</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
@@ -5204,7 +5216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -5220,15 +5232,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
@@ -5698,7 +5710,7 @@
       <c r="C22" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>242</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -5834,16 +5846,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -6575,15 +6587,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -7096,16 +7108,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
@@ -7378,7 +7390,7 @@
       <c r="D12" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>1064</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -7561,8 +7573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7577,15 +7589,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
@@ -7658,22 +7670,22 @@
       <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="29" t="s">
         <v>573</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="29" t="s">
         <v>575</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="29" t="s">
         <v>576</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>577</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="30">
         <v>2018</v>
       </c>
     </row>
@@ -7710,7 +7722,7 @@
       <c r="C7" s="12" t="s">
         <v>583</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>1065</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -8128,8 +8140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8145,16 +8157,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>664</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
@@ -8219,7 +8231,7 @@
       <c r="D4" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>1049</v>
       </c>
       <c r="F4" s="20" t="s">
@@ -8245,7 +8257,7 @@
       <c r="D5" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>1050</v>
       </c>
       <c r="F5" s="20" t="s">
@@ -8271,7 +8283,7 @@
       <c r="D6" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>679</v>
       </c>
       <c r="F6" s="20" t="s">
@@ -8531,7 +8543,7 @@
       <c r="D16" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>1056</v>
       </c>
       <c r="F16" s="20" t="s">
@@ -8739,7 +8751,7 @@
       <c r="D24" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="24" t="s">
         <v>1058</v>
       </c>
       <c r="F24" s="20" t="s">
@@ -8765,7 +8777,7 @@
       <c r="D25" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="24" t="s">
         <v>760</v>
       </c>
       <c r="F25" s="20" t="s">
@@ -8791,7 +8803,7 @@
       <c r="D26" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>1059</v>
       </c>
       <c r="F26" s="20" t="s">
@@ -8819,7 +8831,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8835,16 +8847,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>765</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
@@ -9431,7 +9443,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9447,16 +9459,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>863</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>

</xml_diff>

<commit_message>
update book list and add health check doc
</commit_message>
<xml_diff>
--- a/반월도서관희망도서목록2019.xlsx
+++ b/반월도서관희망도서목록2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\02_Doc\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A25963A-6225-4A6E-A598-620EA9FC9060}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13"/>
+    <workbookView xWindow="2295" yWindow="150" windowWidth="21600" windowHeight="15435" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN1" sheetId="3" r:id="rId1"/>
@@ -26,25 +27,20 @@
     <sheet name="JUN2" sheetId="14" r:id="rId12"/>
     <sheet name="JUL1" sheetId="15" r:id="rId13"/>
     <sheet name="JUL2" sheetId="16" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId15"/>
+    <sheet name="AUG1" sheetId="17" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1722">
   <si>
     <t>반월도서관 1월 1차 희망도서 입수목록(31권)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -4978,17 +4974,282 @@
   </si>
   <si>
     <t>브루노 라투르, 스티브 울거 [공]지음 ; 이상원 옮김</t>
+  </si>
+  <si>
+    <t>반월도서관 8월 1차 희망도서 입수목록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HBM000032932</t>
+  </si>
+  <si>
+    <t>512.49-오65ㅅㅎ</t>
+  </si>
+  <si>
+    <t>(최신)산림치유 개론</t>
+  </si>
+  <si>
+    <t>오오이 겐, 미야자키 요시후미, 히라노 히데키 외 저 ; 한국산림치유포럼 역</t>
+  </si>
+  <si>
+    <t>전나무숲</t>
+  </si>
+  <si>
+    <t>HBM000032933</t>
+  </si>
+  <si>
+    <t>818-손38ㄴ</t>
+  </si>
+  <si>
+    <t>(누가 뭐라고 해도)내가 가는 길이 꽃길이다</t>
+  </si>
+  <si>
+    <t>손미나 지음</t>
+  </si>
+  <si>
+    <t>한빛비즈</t>
+  </si>
+  <si>
+    <t>HBM000032934</t>
+  </si>
+  <si>
+    <t>800.99-슈38ㅁㅎ</t>
+  </si>
+  <si>
+    <t>미친 사랑의 서 : 작가의 밀애, 책 속의 밀어</t>
+  </si>
+  <si>
+    <t>섀넌 매케나 슈미트, 조니 렌던 [공]지음 ; 허형은 옮김</t>
+  </si>
+  <si>
+    <t>HBM000032935</t>
+  </si>
+  <si>
+    <t>005.133-윤68ㅎ</t>
+  </si>
+  <si>
+    <t>혼자 공부하는 파이썬</t>
+  </si>
+  <si>
+    <t>윤인성 지음</t>
+  </si>
+  <si>
+    <t>한빛미디어</t>
+  </si>
+  <si>
+    <t>HBM000032936</t>
+  </si>
+  <si>
+    <t>005.133-이57ㅊ</t>
+  </si>
+  <si>
+    <t>(코딩초보를 위한)72시간 파이썬 정복</t>
+  </si>
+  <si>
+    <t>이승현 [외]공저</t>
+  </si>
+  <si>
+    <t>광문각</t>
+  </si>
+  <si>
+    <t>HBM000032937</t>
+  </si>
+  <si>
+    <t>005.133-이94ㅁ</t>
+  </si>
+  <si>
+    <t>모두의 C언어</t>
+  </si>
+  <si>
+    <t>이형우 지음</t>
+  </si>
+  <si>
+    <t>HBM000032938</t>
+  </si>
+  <si>
+    <t>005.138-한74ㅊ</t>
+  </si>
+  <si>
+    <t>최신 Java 프로그래밍</t>
+  </si>
+  <si>
+    <t>한정란 著</t>
+  </si>
+  <si>
+    <t>21세기사</t>
+  </si>
+  <si>
+    <t>HBM000032939</t>
+  </si>
+  <si>
+    <t>814.7-김63ㅇ</t>
+  </si>
+  <si>
+    <t>잊기 좋은 이름 : 김애란 산문</t>
+  </si>
+  <si>
+    <t>김애란 지음</t>
+  </si>
+  <si>
+    <t>열림원</t>
+  </si>
+  <si>
+    <t>HBM000032940</t>
+  </si>
+  <si>
+    <t>326.79-김14ㅇ</t>
+  </si>
+  <si>
+    <t>유튜브로 책 권하는 법</t>
+  </si>
+  <si>
+    <t>김겨울 지음</t>
+  </si>
+  <si>
+    <t>유유</t>
+  </si>
+  <si>
+    <t>HBM000032941</t>
+  </si>
+  <si>
+    <t>410-고38ㅅㄱ</t>
+  </si>
+  <si>
+    <t>(일상의 무기가 되는)수학 초능력 = Math power : 수학의 정리 편</t>
+  </si>
+  <si>
+    <t>고미야마 히로히토 지음 ; 김은혜 옮김</t>
+  </si>
+  <si>
+    <t>HBM000032942</t>
+  </si>
+  <si>
+    <t>833.6-나87ㅅㄱ</t>
+  </si>
+  <si>
+    <t>산월기 : 나카지마 아쓰시 단편선</t>
+  </si>
+  <si>
+    <t>나카지마 아쓰시 지음 ; 김영식 옮김</t>
+  </si>
+  <si>
+    <t>문예</t>
+  </si>
+  <si>
+    <t>HBM000032943</t>
+  </si>
+  <si>
+    <t>813.7-황74ㄱ</t>
+  </si>
+  <si>
+    <t>계속해보겠습니다 : 황정은 장편소설</t>
+  </si>
+  <si>
+    <t>황정은 지음</t>
+  </si>
+  <si>
+    <t>HBM000032944</t>
+  </si>
+  <si>
+    <t>913.07-톨29ㅇㅂ</t>
+  </si>
+  <si>
+    <t>일본 제국 패망사 : 태평양전쟁 1936~1945</t>
+  </si>
+  <si>
+    <t>존 톨런드 지음 ; 박병화, 이두영 [공]옮김</t>
+  </si>
+  <si>
+    <t>HBM000032945</t>
+  </si>
+  <si>
+    <t>512.49-조44ㅅ</t>
+  </si>
+  <si>
+    <t>4대 만성병 자연치유 교과서</t>
+  </si>
+  <si>
+    <t>조병식 지음</t>
+  </si>
+  <si>
+    <t>왕의서재</t>
+  </si>
+  <si>
+    <t>HBM000032946</t>
+  </si>
+  <si>
+    <t>070.41-이73ㄱ</t>
+  </si>
+  <si>
+    <t>기사 작성의 기초</t>
+  </si>
+  <si>
+    <t>이재경, 송성근 [공]지음</t>
+  </si>
+  <si>
+    <t>이화여자대학교출판문화원</t>
+  </si>
+  <si>
+    <t>HBM000032947</t>
+  </si>
+  <si>
+    <t>337.1-소72ㅇㅇ</t>
+  </si>
+  <si>
+    <t>여자는 왜 완벽하려고 애쓸까</t>
+  </si>
+  <si>
+    <t>레시마 소자니 지음 ; 이미정 옮김</t>
+  </si>
+  <si>
+    <t>HBM000032948</t>
+  </si>
+  <si>
+    <t>853-피83ㄴㅂ</t>
+  </si>
+  <si>
+    <t>내가 죽어야 하는 밤 : 제바스티안 피체크 장편소설</t>
+  </si>
+  <si>
+    <t>제바스티안 피체크 지음 ; 배명자 옮김</t>
+  </si>
+  <si>
+    <t>HBM000032949</t>
+  </si>
+  <si>
+    <t>381.79-모29ㅁㅇ</t>
+  </si>
+  <si>
+    <t>매일매일 좋은 날</t>
+  </si>
+  <si>
+    <t>모리시타 노리코 지음 ; 이유라 옮김</t>
+  </si>
+  <si>
+    <t>HBM000032950</t>
+  </si>
+  <si>
+    <t>491.51-도87ㅇㅎ</t>
+  </si>
+  <si>
+    <t>이기적 유전자</t>
+  </si>
+  <si>
+    <t>리처드 도킨스 지음 ; 홍영남, 이상임 [공]옮김</t>
+  </si>
+  <si>
+    <t>을유문화사</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -4997,14 +5258,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -5013,7 +5274,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -5243,9 +5504,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5254,6 +5512,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5568,7 +5829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -5578,29 +5839,29 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.875" customWidth="1"/>
-    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -5621,7 +5882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -5644,7 +5905,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -5667,7 +5928,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -5690,7 +5951,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -5713,7 +5974,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -5736,7 +5997,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -5759,7 +6020,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -5782,7 +6043,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -5805,7 +6066,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -5828,7 +6089,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -5851,7 +6112,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -5874,7 +6135,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -5897,7 +6158,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -5920,7 +6181,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -5943,7 +6204,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -5966,7 +6227,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -5989,7 +6250,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -6012,7 +6273,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -6035,7 +6296,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -6058,7 +6319,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -6081,7 +6342,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -6104,7 +6365,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -6127,7 +6388,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -6150,7 +6411,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -6173,7 +6434,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -6196,7 +6457,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -6219,7 +6480,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -6242,7 +6503,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -6265,7 +6526,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -6288,7 +6549,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -6311,7 +6572,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -6345,7 +6606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -6355,31 +6616,31 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.75" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="89.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.125" customWidth="1"/>
-    <col min="7" max="7" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="24" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>962</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -6403,7 +6664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -6429,7 +6690,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -6455,7 +6716,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -6481,7 +6742,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -6507,7 +6768,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -6533,7 +6794,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -6559,7 +6820,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -6585,7 +6846,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -6611,7 +6872,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -6637,7 +6898,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -6663,7 +6924,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -6689,7 +6950,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -6715,7 +6976,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -6741,7 +7002,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -6767,7 +7028,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -6793,7 +7054,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -6819,7 +7080,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -6845,7 +7106,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -6871,7 +7132,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="21">
         <v>19</v>
       </c>
@@ -6897,7 +7158,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="21">
         <v>20</v>
       </c>
@@ -6934,7 +7195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -6944,30 +7205,30 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.25" customWidth="1"/>
+    <col min="6" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>1066</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>1</v>
@@ -6991,7 +7252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -7017,7 +7278,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -7043,7 +7304,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -7069,7 +7330,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -7095,7 +7356,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -7121,7 +7382,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -7147,7 +7408,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -7173,7 +7434,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -7199,7 +7460,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -7225,7 +7486,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -7251,7 +7512,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -7277,7 +7538,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -7303,7 +7564,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -7329,7 +7590,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -7355,7 +7616,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -7381,7 +7642,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -7407,7 +7668,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -7433,7 +7694,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -7459,7 +7720,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -7496,7 +7757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -7506,31 +7767,31 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="29.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="97.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="34.5" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>1156</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>1</v>
@@ -7554,7 +7815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -7580,7 +7841,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -7606,7 +7867,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -7632,7 +7893,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -7658,7 +7919,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -7684,7 +7945,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -7710,7 +7971,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -7736,7 +7997,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -7762,7 +8023,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -7788,7 +8049,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -7814,7 +8075,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -7840,7 +8101,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -7866,7 +8127,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -7892,7 +8153,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -7918,7 +8179,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -7944,7 +8205,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -7970,7 +8231,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -7996,7 +8257,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -8022,7 +8283,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -8048,7 +8309,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -8074,7 +8335,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -8100,7 +8361,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -8126,7 +8387,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -8152,7 +8413,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -8178,7 +8439,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -8204,7 +8465,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -8230,7 +8491,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -8256,7 +8517,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -8282,7 +8543,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -8319,7 +8580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -8329,31 +8590,31 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="77" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>1287</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -8377,7 +8638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -8403,7 +8664,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -8429,7 +8690,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -8455,7 +8716,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -8481,7 +8742,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -8507,7 +8768,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -8533,7 +8794,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -8559,7 +8820,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -8585,7 +8846,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -8611,7 +8872,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -8637,7 +8898,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -8663,7 +8924,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -8689,7 +8950,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -8715,7 +8976,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -8741,7 +9002,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -8767,7 +9028,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -8793,7 +9054,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -8819,7 +9080,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -8845,7 +9106,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -8871,7 +9132,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -8897,7 +9158,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -8923,7 +9184,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -8949,7 +9210,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -8975,7 +9236,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -9001,7 +9262,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="20">
         <v>25</v>
       </c>
@@ -9027,7 +9288,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="20">
         <v>26</v>
       </c>
@@ -9053,7 +9314,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="20">
         <v>27</v>
       </c>
@@ -9079,7 +9340,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="20">
         <v>28</v>
       </c>
@@ -9105,7 +9366,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="20">
         <v>29</v>
       </c>
@@ -9131,7 +9392,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="20">
         <v>30</v>
       </c>
@@ -9157,7 +9418,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="20">
         <v>31</v>
       </c>
@@ -9183,7 +9444,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="20">
         <v>32</v>
       </c>
@@ -9220,38 +9481,38 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.125" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>1430</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -9275,7 +9536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -9301,7 +9562,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -9327,7 +9588,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -9353,7 +9614,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -9379,7 +9640,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -9405,7 +9666,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -9431,7 +9692,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -9457,7 +9718,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -9483,7 +9744,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -9509,7 +9770,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -9535,7 +9796,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -9561,7 +9822,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -9587,7 +9848,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -9613,7 +9874,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -9639,7 +9900,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -9665,7 +9926,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -9691,7 +9952,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -9717,7 +9978,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -9743,7 +10004,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -9769,7 +10030,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -9795,7 +10056,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -9821,7 +10082,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -9847,7 +10108,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -9873,7 +10134,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -9899,7 +10160,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="20">
         <v>25</v>
       </c>
@@ -9925,7 +10186,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="20">
         <v>26</v>
       </c>
@@ -9951,7 +10212,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="20">
         <v>27</v>
       </c>
@@ -9977,7 +10238,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="20">
         <v>28</v>
       </c>
@@ -10003,7 +10264,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="20">
         <v>29</v>
       </c>
@@ -10029,7 +10290,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="20">
         <v>30</v>
       </c>
@@ -10055,7 +10316,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="20">
         <v>31</v>
       </c>
@@ -10081,7 +10342,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="20">
         <v>32</v>
       </c>
@@ -10107,7 +10368,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="20">
         <v>33</v>
       </c>
@@ -10133,7 +10394,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="20">
         <v>34</v>
       </c>
@@ -10159,7 +10420,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="20">
         <v>35</v>
       </c>
@@ -10185,7 +10446,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="20">
         <v>36</v>
       </c>
@@ -10211,7 +10472,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="20">
         <v>37</v>
       </c>
@@ -10237,7 +10498,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="20">
         <v>38</v>
       </c>
@@ -10263,7 +10524,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" s="20">
         <v>39</v>
       </c>
@@ -10289,7 +10550,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="20">
         <v>40</v>
       </c>
@@ -10315,7 +10576,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="20">
         <v>41</v>
       </c>
@@ -10341,7 +10602,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="20">
         <v>42</v>
       </c>
@@ -10367,7 +10628,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="20">
         <v>43</v>
       </c>
@@ -10393,7 +10654,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="20">
         <v>44</v>
       </c>
@@ -10419,7 +10680,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="20">
         <v>45</v>
       </c>
@@ -10445,7 +10706,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="20">
         <v>46</v>
       </c>
@@ -10482,14 +10743,576 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6DE92A-8DF2-43F1-8092-3558ADD8367D}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1636</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1637</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>1638</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>1642</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>1643</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>1647</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>1648</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>1651</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>1652</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>1653</v>
+      </c>
+      <c r="H6" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1656</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>1657</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>1658</v>
+      </c>
+      <c r="H7" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1660</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>1661</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>1662</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>1665</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>1666</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>1667</v>
+      </c>
+      <c r="H9" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>1669</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>1672</v>
+      </c>
+      <c r="H10" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H11" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>1680</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>1681</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>818</v>
+      </c>
+      <c r="H12" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A13" s="11">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>1684</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>1686</v>
+      </c>
+      <c r="H13" s="11">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A14" s="11">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>1690</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="H14" s="11">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A15" s="11">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>1693</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>1694</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>862</v>
+      </c>
+      <c r="H15" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>1697</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>1698</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>1699</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A17" s="11">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>1704</v>
+      </c>
+      <c r="H17" s="11">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A18" s="11">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>1707</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>1708</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A19" s="11">
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>1711</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>1712</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A20" s="11">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>1716</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A21" s="11">
+        <v>19</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>1720</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>1721</v>
+      </c>
+      <c r="H21" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10497,7 +11320,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -10507,29 +11330,29 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -10550,7 +11373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -10573,7 +11396,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="20.25" customHeight="1">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -10596,7 +11419,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="20.25" customHeight="1">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -10619,7 +11442,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="20.25" customHeight="1">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -10642,7 +11465,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="20.25" customHeight="1">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -10665,7 +11488,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="20.25" customHeight="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -10688,7 +11511,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="20.25" customHeight="1">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -10711,7 +11534,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="20.25" customHeight="1">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -10734,7 +11557,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="20.25" customHeight="1">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -10757,7 +11580,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="20.25" customHeight="1">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -10780,7 +11603,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="20.25" customHeight="1">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -10803,7 +11626,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="20.25" customHeight="1">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -10826,7 +11649,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="20.25" customHeight="1">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -10849,7 +11672,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="20.25" customHeight="1">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -10872,7 +11695,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="20.25" customHeight="1">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -10895,7 +11718,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="20.25" customHeight="1">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -10918,7 +11741,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="20.25" customHeight="1">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -10941,7 +11764,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="20.25" customHeight="1">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -10964,7 +11787,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="20.25" customHeight="1">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -10987,7 +11810,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="20.25" customHeight="1">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -10997,7 +11820,7 @@
       <c r="C22" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="31" t="s">
         <v>242</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -11010,7 +11833,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="20.25" customHeight="1">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -11033,7 +11856,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="20.25" customHeight="1">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -11056,7 +11879,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="20.25" customHeight="1">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -11079,7 +11902,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="20.25" customHeight="1">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -11113,7 +11936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -11123,31 +11946,31 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="70.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="36.75" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>1</v>
@@ -11171,7 +11994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18" customHeight="1">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -11197,7 +12020,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -11223,7 +12046,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -11249,7 +12072,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -11275,7 +12098,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -11301,7 +12124,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -11327,7 +12150,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -11353,7 +12176,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -11379,7 +12202,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -11405,7 +12228,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -11431,7 +12254,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -11457,7 +12280,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -11483,7 +12306,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -11509,7 +12332,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -11535,7 +12358,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -11561,7 +12384,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -11587,7 +12410,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -11613,7 +12436,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -11639,7 +12462,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -11665,7 +12488,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="11">
         <v>20</v>
       </c>
@@ -11691,7 +12514,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -11717,7 +12540,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -11743,7 +12566,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -11769,7 +12592,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -11795,7 +12618,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="11">
         <v>25</v>
       </c>
@@ -11821,7 +12644,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -11858,7 +12681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -11868,29 +12691,29 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>1</v>
@@ -11911,7 +12734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -11934,7 +12757,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -11957,7 +12780,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18" customHeight="1">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -11980,7 +12803,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" customHeight="1">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -12003,7 +12826,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18" customHeight="1">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -12026,7 +12849,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18" customHeight="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -12049,7 +12872,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -12072,7 +12895,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -12095,7 +12918,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -12118,7 +12941,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18" customHeight="1">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -12141,7 +12964,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" customHeight="1">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -12164,7 +12987,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" customHeight="1">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -12187,7 +13010,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18" customHeight="1">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -12210,7 +13033,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18" customHeight="1">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -12233,7 +13056,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18" customHeight="1">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -12256,7 +13079,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18" customHeight="1">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -12279,7 +13102,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="18" customHeight="1">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -12302,7 +13125,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="18" customHeight="1">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -12325,7 +13148,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="18" customHeight="1">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -12348,7 +13171,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="18" customHeight="1">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -12382,7 +13205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -12392,30 +13215,30 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="56.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="27" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="14"/>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -12439,7 +13262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18" customHeight="1">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -12465,7 +13288,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -12491,7 +13314,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18" customHeight="1">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -12517,7 +13340,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18" customHeight="1">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -12543,7 +13366,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18" customHeight="1">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -12569,7 +13392,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18" customHeight="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -12595,7 +13418,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18" customHeight="1">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -12621,7 +13444,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18" customHeight="1">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -12647,7 +13470,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18" customHeight="1">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -12673,7 +13496,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" customHeight="1">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -12699,7 +13522,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18" customHeight="1">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -12725,7 +13548,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18" customHeight="1">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -12751,7 +13574,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" customHeight="1">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -12777,7 +13600,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" customHeight="1">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -12803,7 +13626,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" customHeight="1">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -12829,7 +13652,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" customHeight="1">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -12866,7 +13689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -12876,29 +13699,29 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.25" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
         <v>1</v>
@@ -12919,7 +13742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -12942,7 +13765,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -12965,7 +13788,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -12988,7 +13811,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -13011,7 +13834,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -13034,7 +13857,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -13057,7 +13880,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -13080,7 +13903,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -13103,7 +13926,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -13126,7 +13949,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -13149,7 +13972,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -13172,7 +13995,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -13195,7 +14018,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -13218,7 +14041,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -13241,7 +14064,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -13264,7 +14087,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -13287,7 +14110,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -13310,7 +14133,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -13333,7 +14156,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -13356,7 +14179,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1">
       <c r="A22" s="11">
         <v>20</v>
       </c>
@@ -13379,7 +14202,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -13402,7 +14225,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -13436,7 +14259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -13446,31 +14269,31 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="59.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="34" t="s">
         <v>664</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -13494,7 +14317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="17.25" customHeight="1">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -13520,7 +14343,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="17.25" customHeight="1">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -13533,7 +14356,7 @@
       <c r="D4" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>1049</v>
       </c>
       <c r="F4" s="20" t="s">
@@ -13546,7 +14369,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -13572,7 +14395,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="17.25" customHeight="1">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -13598,7 +14421,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="17.25" customHeight="1">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -13624,7 +14447,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="17.25" customHeight="1">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -13650,7 +14473,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="17.25" customHeight="1">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -13676,7 +14499,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="17.25" customHeight="1">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -13702,7 +14525,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="17.25" customHeight="1">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -13728,7 +14551,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="17.25" customHeight="1">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -13754,7 +14577,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17.25" customHeight="1">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -13780,7 +14603,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="17.25" customHeight="1">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -13806,7 +14629,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="17.25" customHeight="1">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -13832,7 +14655,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="17.25" customHeight="1">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -13845,7 +14668,7 @@
       <c r="D16" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="32" t="s">
         <v>1056</v>
       </c>
       <c r="F16" s="20" t="s">
@@ -13858,7 +14681,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="17.25" customHeight="1">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -13884,7 +14707,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="17.25" customHeight="1">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -13910,7 +14733,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="17.25" customHeight="1">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -13936,7 +14759,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="17.25" customHeight="1">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -13962,7 +14785,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="17.25" customHeight="1">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -13988,7 +14811,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="17.25" customHeight="1">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -14014,7 +14837,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="17.25" customHeight="1">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -14040,7 +14863,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="17.25" customHeight="1">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -14066,7 +14889,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="17.25" customHeight="1">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -14092,7 +14915,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="17.25" customHeight="1">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -14129,7 +14952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -14139,31 +14962,31 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="5" max="5" width="64.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.75" customWidth="1"/>
-    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="25.5" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>765</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -14187,7 +15010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="19.5" customHeight="1">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -14213,7 +15036,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="19.5" customHeight="1">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -14239,7 +15062,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="19.5" customHeight="1">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -14265,7 +15088,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -14278,7 +15101,7 @@
       <c r="D6" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="33" t="s">
         <v>781</v>
       </c>
       <c r="F6" s="23" t="s">
@@ -14291,7 +15114,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="19.5" customHeight="1">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -14317,7 +15140,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -14343,7 +15166,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="19.5" customHeight="1">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -14369,7 +15192,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -14395,7 +15218,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
       <c r="A11" s="22">
         <v>9</v>
       </c>
@@ -14421,7 +15244,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="19.5" customHeight="1">
       <c r="A12" s="22">
         <v>10</v>
       </c>
@@ -14434,7 +15257,7 @@
       <c r="D12" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="33" t="s">
         <v>807</v>
       </c>
       <c r="F12" s="23" t="s">
@@ -14447,7 +15270,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="19.5" customHeight="1">
       <c r="A13" s="22">
         <v>11</v>
       </c>
@@ -14473,7 +15296,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="19.5" customHeight="1">
       <c r="A14" s="22">
         <v>12</v>
       </c>
@@ -14499,7 +15322,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="19.5" customHeight="1">
       <c r="A15" s="22">
         <v>13</v>
       </c>
@@ -14525,7 +15348,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="19.5" customHeight="1">
       <c r="A16" s="22">
         <v>14</v>
       </c>
@@ -14551,7 +15374,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="19.5" customHeight="1">
       <c r="A17" s="22">
         <v>15</v>
       </c>
@@ -14577,7 +15400,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="19.5" customHeight="1">
       <c r="A18" s="22">
         <v>16</v>
       </c>
@@ -14603,7 +15426,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="19.5" customHeight="1">
       <c r="A19" s="22">
         <v>17</v>
       </c>
@@ -14629,7 +15452,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="19.5" customHeight="1">
       <c r="A20" s="22">
         <v>18</v>
       </c>
@@ -14655,7 +15478,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="19.5" customHeight="1">
       <c r="A21" s="22">
         <v>19</v>
       </c>
@@ -14681,7 +15504,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="19.5" customHeight="1">
       <c r="A22" s="22">
         <v>20</v>
       </c>
@@ -14707,7 +15530,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="19.5" customHeight="1">
       <c r="A23" s="22">
         <v>21</v>
       </c>
@@ -14744,7 +15567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -14754,31 +15577,31 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="54.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="27" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>863</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -14802,7 +15625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -14828,7 +15651,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -14854,7 +15677,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -14880,7 +15703,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -14906,7 +15729,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -14932,7 +15755,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -14958,7 +15781,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -14984,7 +15807,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -15010,7 +15833,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -15036,7 +15859,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -15062,7 +15885,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -15088,7 +15911,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -15114,7 +15937,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -15140,7 +15963,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -15166,7 +15989,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -15192,7 +16015,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -15218,7 +16041,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -15244,7 +16067,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -15257,7 +16080,7 @@
       <c r="D20" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>944</v>
       </c>
       <c r="F20" s="20" t="s">
@@ -15270,7 +16093,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="21">
         <v>19</v>
       </c>
@@ -15296,7 +16119,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="21">
         <v>20</v>
       </c>
@@ -15322,7 +16145,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="21">
         <v>21</v>
       </c>

</xml_diff>